<commit_message>
minor changes to the pbaseniorusopen2024 excel file
</commit_message>
<xml_diff>
--- a/inst/extdata/PBASeniorUSOpen2024_finalstandings.xlsx
+++ b/inst/extdata/PBASeniorUSOpen2024_finalstandings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PBAData\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PBAData\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92C244F0-23AE-4D6E-94E6-88A2D51633C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5B2947-CBC0-413A-8330-2FD66947CB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{50E31A33-E17E-4874-9437-CFBA9816E013}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50E31A33-E17E-4874-9437-CFBA9816E013}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,97 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="153">
-  <si>
-    <t>$15,000</t>
-  </si>
-  <si>
-    <t>$8,000</t>
-  </si>
-  <si>
-    <t>$6,000</t>
-  </si>
-  <si>
-    <t>$5,000</t>
-  </si>
-  <si>
-    <t>$4,000</t>
-  </si>
-  <si>
-    <t>$3,000</t>
-  </si>
-  <si>
-    <t>$2,500</t>
-  </si>
-  <si>
-    <t>$2,400</t>
-  </si>
-  <si>
-    <t>$2,300</t>
-  </si>
-  <si>
-    <t>$2,200</t>
-  </si>
-  <si>
-    <t>$2,100</t>
-  </si>
-  <si>
-    <t>$2,000</t>
-  </si>
-  <si>
-    <t>$1,950</t>
-  </si>
-  <si>
-    <t>$1,900</t>
-  </si>
-  <si>
-    <t>$1,850</t>
-  </si>
-  <si>
-    <t>$1,800</t>
-  </si>
-  <si>
-    <t>$1,750</t>
-  </si>
-  <si>
-    <t>$1,700</t>
-  </si>
-  <si>
-    <t>$1,650</t>
-  </si>
-  <si>
-    <t>$1,600</t>
-  </si>
-  <si>
-    <t>$1,550</t>
-  </si>
-  <si>
-    <t>$1,500</t>
-  </si>
-  <si>
-    <t>$1,450</t>
-  </si>
-  <si>
-    <t>$1,400</t>
-  </si>
-  <si>
-    <t>$1,225</t>
-  </si>
-  <si>
-    <t>$1,187.50</t>
-  </si>
-  <si>
-    <t>$1,150</t>
-  </si>
-  <si>
-    <t>$1,050</t>
-  </si>
-  <si>
-    <t>$120</t>
-  </si>
-  <si>
-    <t>$525</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>John Janawicz</t>
   </si>
@@ -490,6 +400,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,9 +432,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,54 +754,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8F7F13-0E2B-4A9C-82B6-2A84134B809B}">
   <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H1" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="I1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>9992</v>
@@ -908,13 +824,13 @@
       <c r="H2">
         <v>2500</v>
       </c>
-      <c r="I2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>9499</v>
@@ -937,13 +853,13 @@
       <c r="H3">
         <v>1500</v>
       </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>9531</v>
@@ -966,13 +882,13 @@
       <c r="H4">
         <v>1150</v>
       </c>
-      <c r="I4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>9487</v>
@@ -995,13 +911,13 @@
       <c r="H5">
         <v>950</v>
       </c>
-      <c r="I5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5" s="2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>9404</v>
@@ -1024,13 +940,13 @@
       <c r="H6">
         <v>850</v>
       </c>
-      <c r="I6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>8931</v>
@@ -1053,13 +969,13 @@
       <c r="H7">
         <v>775</v>
       </c>
-      <c r="I7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>8949</v>
@@ -1082,13 +998,13 @@
       <c r="H8">
         <v>745</v>
       </c>
-      <c r="I8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>8837</v>
@@ -1111,13 +1027,13 @@
       <c r="H9">
         <v>715</v>
       </c>
-      <c r="I9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>8863</v>
@@ -1140,13 +1056,13 @@
       <c r="H10">
         <v>685</v>
       </c>
-      <c r="I10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>8845</v>
@@ -1169,13 +1085,13 @@
       <c r="H11">
         <v>655</v>
       </c>
-      <c r="I11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>8820</v>
@@ -1198,13 +1114,13 @@
       <c r="H12">
         <v>625</v>
       </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>8906</v>
@@ -1227,13 +1143,13 @@
       <c r="H13">
         <v>595</v>
       </c>
-      <c r="I13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>8879</v>
@@ -1256,13 +1172,13 @@
       <c r="H14">
         <v>565</v>
       </c>
-      <c r="I14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>8750</v>
@@ -1285,13 +1201,13 @@
       <c r="H15">
         <v>535</v>
       </c>
-      <c r="I15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>8699</v>
@@ -1314,13 +1230,13 @@
       <c r="H16">
         <v>505</v>
       </c>
-      <c r="I16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>8674</v>
@@ -1343,13 +1259,13 @@
       <c r="H17">
         <v>475</v>
       </c>
-      <c r="I17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>8585</v>
@@ -1372,13 +1288,13 @@
       <c r="H18">
         <v>445</v>
       </c>
-      <c r="I18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>8601</v>
@@ -1401,13 +1317,13 @@
       <c r="H19">
         <v>425</v>
       </c>
-      <c r="I19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>8546</v>
@@ -1430,13 +1346,13 @@
       <c r="H20">
         <v>405</v>
       </c>
-      <c r="I20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>8498</v>
@@ -1459,13 +1375,13 @@
       <c r="H21">
         <v>385</v>
       </c>
-      <c r="I21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>8484</v>
@@ -1488,13 +1404,13 @@
       <c r="H22">
         <v>365</v>
       </c>
-      <c r="I22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="2">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>8437</v>
@@ -1517,13 +1433,13 @@
       <c r="H23">
         <v>345</v>
       </c>
-      <c r="I23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>8419</v>
@@ -1546,13 +1462,13 @@
       <c r="H24">
         <v>325</v>
       </c>
-      <c r="I24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="2">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>8478</v>
@@ -1575,13 +1491,13 @@
       <c r="H25">
         <v>305</v>
       </c>
-      <c r="I25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="2">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>3660</v>
@@ -1604,13 +1520,13 @@
       <c r="H26">
         <v>285</v>
       </c>
-      <c r="I26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="2">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>3656</v>
@@ -1633,13 +1549,13 @@
       <c r="H27">
         <v>275</v>
       </c>
-      <c r="I27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="2">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>3654</v>
@@ -1662,13 +1578,13 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="2">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>3645</v>
@@ -1691,13 +1607,13 @@
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="I29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="2">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>3643</v>
@@ -1720,13 +1636,13 @@
       <c r="H30">
         <v>245</v>
       </c>
-      <c r="I30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="2">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>3641</v>
@@ -1749,13 +1665,13 @@
       <c r="H31">
         <v>235</v>
       </c>
-      <c r="I31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="2">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>3637</v>
@@ -1778,13 +1694,13 @@
       <c r="H32">
         <v>225</v>
       </c>
-      <c r="I32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="2">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>3630</v>
@@ -1807,13 +1723,13 @@
       <c r="H33">
         <v>215</v>
       </c>
-      <c r="I33" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="4">
+        <v>1187.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>3630</v>
@@ -1836,13 +1752,13 @@
       <c r="H34">
         <v>205</v>
       </c>
-      <c r="I34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="4">
+        <v>1187.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>3625</v>
@@ -1865,13 +1781,13 @@
       <c r="H35">
         <v>200</v>
       </c>
-      <c r="I35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="2">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>3623</v>
@@ -1894,13 +1810,13 @@
       <c r="H36">
         <v>195</v>
       </c>
-      <c r="I36" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="2">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>3621</v>
@@ -1923,13 +1839,13 @@
       <c r="H37">
         <v>190</v>
       </c>
-      <c r="I37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="2">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>3620</v>
@@ -1952,13 +1868,13 @@
       <c r="H38">
         <v>185</v>
       </c>
-      <c r="I38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="2">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>3618</v>
@@ -1981,13 +1897,13 @@
       <c r="H39">
         <v>180</v>
       </c>
-      <c r="I39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="2">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>3608</v>
@@ -2010,13 +1926,13 @@
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="2">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>3607</v>
@@ -2040,9 +1956,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>3607</v>
@@ -2066,9 +1982,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>3605</v>
@@ -2091,13 +2007,13 @@
       <c r="H43">
         <v>160</v>
       </c>
-      <c r="I43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="2">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>3589</v>
@@ -2120,13 +2036,13 @@
       <c r="H44">
         <v>155</v>
       </c>
-      <c r="I44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="2">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>3573</v>
@@ -2150,9 +2066,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>3570</v>
@@ -2176,9 +2092,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>3563</v>
@@ -2202,9 +2118,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>3562</v>
@@ -2228,9 +2144,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>3554</v>
@@ -2253,13 +2169,13 @@
       <c r="H49">
         <v>0</v>
       </c>
-      <c r="I49" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="2">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>3554</v>
@@ -2283,9 +2199,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>3553</v>
@@ -2309,9 +2225,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>3552</v>
@@ -2335,9 +2251,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>3530</v>
@@ -2360,13 +2276,13 @@
       <c r="H53">
         <v>110</v>
       </c>
-      <c r="I53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="2">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>3524</v>
@@ -2390,9 +2306,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>3522</v>
@@ -2416,9 +2332,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>3521</v>
@@ -2441,13 +2357,13 @@
       <c r="H56">
         <v>95</v>
       </c>
-      <c r="I56" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="2">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>3502</v>
@@ -2471,9 +2387,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>3490</v>
@@ -2497,9 +2413,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>3489</v>
@@ -2522,13 +2438,13 @@
       <c r="H59">
         <v>80</v>
       </c>
-      <c r="I59" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I59" s="2">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>3483</v>
@@ -2552,9 +2468,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>3479</v>
@@ -2578,9 +2494,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>3477</v>
@@ -2604,9 +2520,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>3470</v>
@@ -2630,9 +2546,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>3463</v>
@@ -2656,9 +2572,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>3456</v>
@@ -2682,9 +2598,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>3450</v>
@@ -2708,9 +2624,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>3444</v>
@@ -2734,9 +2650,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="B68">
         <v>3443</v>
@@ -2760,9 +2676,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="B69">
         <v>3442</v>
@@ -2785,13 +2701,13 @@
       <c r="H69">
         <v>45</v>
       </c>
-      <c r="I69" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="B70">
         <v>3432</v>
@@ -2815,9 +2731,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="B71">
         <v>3432</v>
@@ -2841,9 +2757,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B72">
         <v>3432</v>
@@ -2867,9 +2783,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="B73">
         <v>3427</v>
@@ -2893,9 +2809,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="B74">
         <v>3426</v>
@@ -2919,9 +2835,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="B75">
         <v>3422</v>
@@ -2945,9 +2861,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="B76">
         <v>3421</v>
@@ -2971,9 +2887,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="B77">
         <v>3410</v>
@@ -2997,9 +2913,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="B78">
         <v>3406</v>
@@ -3023,9 +2939,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="B79">
         <v>3405</v>
@@ -3048,13 +2964,13 @@
       <c r="H79">
         <v>0</v>
       </c>
-      <c r="I79" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>3390</v>
@@ -3078,9 +2994,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="B81">
         <v>3383</v>
@@ -3104,9 +3020,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="B82">
         <v>3377</v>
@@ -3130,9 +3046,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B83">
         <v>3349</v>
@@ -3156,9 +3072,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B84">
         <v>3348</v>
@@ -3182,9 +3098,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="B85">
         <v>3334</v>
@@ -3208,9 +3124,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="B86">
         <v>3329</v>
@@ -3234,9 +3150,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B87">
         <v>3323</v>
@@ -3260,9 +3176,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B88">
         <v>3320</v>
@@ -3285,13 +3201,13 @@
       <c r="H88">
         <v>45</v>
       </c>
-      <c r="I88" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="B89">
         <v>3288</v>
@@ -3315,9 +3231,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>3283</v>
@@ -3341,9 +3257,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>3279</v>
@@ -3367,9 +3283,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>3272</v>
@@ -3393,9 +3309,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>3236</v>
@@ -3419,9 +3335,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>3232</v>
@@ -3445,9 +3361,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>3210</v>
@@ -3471,9 +3387,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="B96">
         <v>3206</v>
@@ -3497,9 +3413,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="B97">
         <v>3191</v>
@@ -3523,9 +3439,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="B98">
         <v>3187</v>
@@ -3549,9 +3465,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="B99">
         <v>3183</v>
@@ -3575,9 +3491,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>3154</v>
@@ -3601,9 +3517,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>3154</v>
@@ -3627,9 +3543,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>3144</v>
@@ -3653,9 +3569,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="B103">
         <v>3131</v>
@@ -3679,9 +3595,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="B104">
         <v>3089</v>
@@ -3705,9 +3621,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="B105">
         <v>3084</v>
@@ -3731,9 +3647,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="B106">
         <v>3066</v>
@@ -3757,9 +3673,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="B107">
         <v>3031</v>
@@ -3783,9 +3699,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="B108">
         <v>3026</v>
@@ -3809,9 +3725,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="B109">
         <v>3008</v>
@@ -3835,9 +3751,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="B110">
         <v>2841</v>
@@ -3861,9 +3777,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B111">
         <v>2783</v>
@@ -3887,9 +3803,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="B112">
         <v>2363</v>
@@ -3913,9 +3829,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="B113">
         <v>1401</v>
@@ -3939,9 +3855,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="B114">
         <v>1321</v>
@@ -3965,9 +3881,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="B115">
         <v>1109</v>

</xml_diff>